<commit_message>
Made all buttons functional
</commit_message>
<xml_diff>
--- a/clustering_result_Mall_Customers.xlsx
+++ b/clustering_result_Mall_Customers.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -467,10 +467,8 @@
       <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C2" t="n">
+        <v>19</v>
       </c>
       <c r="D2" t="n">
         <v>15</v>
@@ -489,10 +487,8 @@
       <c r="B3" t="n">
         <v>2</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C3" t="n">
+        <v>21</v>
       </c>
       <c r="D3" t="n">
         <v>15</v>
@@ -511,10 +507,8 @@
       <c r="B4" t="n">
         <v>3</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C4" t="n">
+        <v>20</v>
       </c>
       <c r="D4" t="n">
         <v>16</v>
@@ -533,10 +527,8 @@
       <c r="B5" t="n">
         <v>4</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C5" t="n">
+        <v>23</v>
       </c>
       <c r="D5" t="n">
         <v>16</v>
@@ -555,10 +547,8 @@
       <c r="B6" t="n">
         <v>5</v>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C6" t="n">
+        <v>31</v>
       </c>
       <c r="D6" t="n">
         <v>17</v>
@@ -577,10 +567,8 @@
       <c r="B7" t="n">
         <v>6</v>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C7" t="n">
+        <v>22</v>
       </c>
       <c r="D7" t="n">
         <v>17</v>
@@ -599,10 +587,8 @@
       <c r="B8" t="n">
         <v>7</v>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C8" t="n">
+        <v>35</v>
       </c>
       <c r="D8" t="n">
         <v>18</v>
@@ -621,10 +607,8 @@
       <c r="B9" t="n">
         <v>8</v>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C9" t="n">
+        <v>23</v>
       </c>
       <c r="D9" t="n">
         <v>18</v>
@@ -633,7 +617,7 @@
         <v>94</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -643,10 +627,8 @@
       <c r="B10" t="n">
         <v>9</v>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C10" t="n">
+        <v>64</v>
       </c>
       <c r="D10" t="n">
         <v>19</v>
@@ -665,10 +647,8 @@
       <c r="B11" t="n">
         <v>10</v>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C11" t="n">
+        <v>30</v>
       </c>
       <c r="D11" t="n">
         <v>19</v>
@@ -687,10 +667,8 @@
       <c r="B12" t="n">
         <v>11</v>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C12" t="n">
+        <v>67</v>
       </c>
       <c r="D12" t="n">
         <v>19</v>
@@ -709,10 +687,8 @@
       <c r="B13" t="n">
         <v>12</v>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C13" t="n">
+        <v>35</v>
       </c>
       <c r="D13" t="n">
         <v>19</v>
@@ -721,7 +697,7 @@
         <v>99</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -731,10 +707,8 @@
       <c r="B14" t="n">
         <v>13</v>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C14" t="n">
+        <v>58</v>
       </c>
       <c r="D14" t="n">
         <v>20</v>
@@ -753,10 +727,8 @@
       <c r="B15" t="n">
         <v>14</v>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C15" t="n">
+        <v>24</v>
       </c>
       <c r="D15" t="n">
         <v>20</v>
@@ -775,10 +747,8 @@
       <c r="B16" t="n">
         <v>15</v>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C16" t="n">
+        <v>37</v>
       </c>
       <c r="D16" t="n">
         <v>20</v>
@@ -797,10 +767,8 @@
       <c r="B17" t="n">
         <v>16</v>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C17" t="n">
+        <v>22</v>
       </c>
       <c r="D17" t="n">
         <v>20</v>
@@ -819,10 +787,8 @@
       <c r="B18" t="n">
         <v>17</v>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C18" t="n">
+        <v>35</v>
       </c>
       <c r="D18" t="n">
         <v>21</v>
@@ -841,10 +807,8 @@
       <c r="B19" t="n">
         <v>18</v>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C19" t="n">
+        <v>20</v>
       </c>
       <c r="D19" t="n">
         <v>21</v>
@@ -863,10 +827,8 @@
       <c r="B20" t="n">
         <v>19</v>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C20" t="n">
+        <v>52</v>
       </c>
       <c r="D20" t="n">
         <v>23</v>
@@ -885,10 +847,8 @@
       <c r="B21" t="n">
         <v>20</v>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C21" t="n">
+        <v>35</v>
       </c>
       <c r="D21" t="n">
         <v>23</v>
@@ -897,7 +857,7 @@
         <v>98</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -907,10 +867,8 @@
       <c r="B22" t="n">
         <v>21</v>
       </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C22" t="n">
+        <v>35</v>
       </c>
       <c r="D22" t="n">
         <v>24</v>
@@ -929,10 +887,8 @@
       <c r="B23" t="n">
         <v>22</v>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C23" t="n">
+        <v>25</v>
       </c>
       <c r="D23" t="n">
         <v>24</v>
@@ -951,10 +907,8 @@
       <c r="B24" t="n">
         <v>23</v>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C24" t="n">
+        <v>46</v>
       </c>
       <c r="D24" t="n">
         <v>25</v>
@@ -973,10 +927,8 @@
       <c r="B25" t="n">
         <v>24</v>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C25" t="n">
+        <v>31</v>
       </c>
       <c r="D25" t="n">
         <v>25</v>
@@ -995,10 +947,8 @@
       <c r="B26" t="n">
         <v>25</v>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C26" t="n">
+        <v>54</v>
       </c>
       <c r="D26" t="n">
         <v>28</v>
@@ -1017,10 +967,8 @@
       <c r="B27" t="n">
         <v>26</v>
       </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C27" t="n">
+        <v>29</v>
       </c>
       <c r="D27" t="n">
         <v>28</v>
@@ -1039,10 +987,8 @@
       <c r="B28" t="n">
         <v>27</v>
       </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C28" t="n">
+        <v>45</v>
       </c>
       <c r="D28" t="n">
         <v>28</v>
@@ -1061,10 +1007,8 @@
       <c r="B29" t="n">
         <v>28</v>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C29" t="n">
+        <v>35</v>
       </c>
       <c r="D29" t="n">
         <v>28</v>
@@ -1083,10 +1027,8 @@
       <c r="B30" t="n">
         <v>29</v>
       </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C30" t="n">
+        <v>40</v>
       </c>
       <c r="D30" t="n">
         <v>29</v>
@@ -1105,10 +1047,8 @@
       <c r="B31" t="n">
         <v>30</v>
       </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C31" t="n">
+        <v>23</v>
       </c>
       <c r="D31" t="n">
         <v>29</v>
@@ -1127,10 +1067,8 @@
       <c r="B32" t="n">
         <v>31</v>
       </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C32" t="n">
+        <v>60</v>
       </c>
       <c r="D32" t="n">
         <v>30</v>
@@ -1149,10 +1087,8 @@
       <c r="B33" t="n">
         <v>32</v>
       </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C33" t="n">
+        <v>21</v>
       </c>
       <c r="D33" t="n">
         <v>30</v>
@@ -1171,10 +1107,8 @@
       <c r="B34" t="n">
         <v>33</v>
       </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C34" t="n">
+        <v>53</v>
       </c>
       <c r="D34" t="n">
         <v>33</v>
@@ -1193,10 +1127,8 @@
       <c r="B35" t="n">
         <v>34</v>
       </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C35" t="n">
+        <v>18</v>
       </c>
       <c r="D35" t="n">
         <v>33</v>
@@ -1215,10 +1147,8 @@
       <c r="B36" t="n">
         <v>35</v>
       </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C36" t="n">
+        <v>49</v>
       </c>
       <c r="D36" t="n">
         <v>33</v>
@@ -1237,10 +1167,8 @@
       <c r="B37" t="n">
         <v>36</v>
       </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C37" t="n">
+        <v>21</v>
       </c>
       <c r="D37" t="n">
         <v>33</v>
@@ -1259,10 +1187,8 @@
       <c r="B38" t="n">
         <v>37</v>
       </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C38" t="n">
+        <v>42</v>
       </c>
       <c r="D38" t="n">
         <v>34</v>
@@ -1281,10 +1207,8 @@
       <c r="B39" t="n">
         <v>38</v>
       </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C39" t="n">
+        <v>30</v>
       </c>
       <c r="D39" t="n">
         <v>34</v>
@@ -1303,10 +1227,8 @@
       <c r="B40" t="n">
         <v>39</v>
       </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C40" t="n">
+        <v>36</v>
       </c>
       <c r="D40" t="n">
         <v>37</v>
@@ -1325,10 +1247,8 @@
       <c r="B41" t="n">
         <v>40</v>
       </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C41" t="n">
+        <v>20</v>
       </c>
       <c r="D41" t="n">
         <v>37</v>
@@ -1347,10 +1267,8 @@
       <c r="B42" t="n">
         <v>41</v>
       </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C42" t="n">
+        <v>65</v>
       </c>
       <c r="D42" t="n">
         <v>38</v>
@@ -1369,10 +1287,8 @@
       <c r="B43" t="n">
         <v>42</v>
       </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C43" t="n">
+        <v>24</v>
       </c>
       <c r="D43" t="n">
         <v>38</v>
@@ -1391,10 +1307,8 @@
       <c r="B44" t="n">
         <v>43</v>
       </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C44" t="n">
+        <v>48</v>
       </c>
       <c r="D44" t="n">
         <v>39</v>
@@ -1413,10 +1327,8 @@
       <c r="B45" t="n">
         <v>44</v>
       </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C45" t="n">
+        <v>31</v>
       </c>
       <c r="D45" t="n">
         <v>39</v>
@@ -1435,10 +1347,8 @@
       <c r="B46" t="n">
         <v>45</v>
       </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C46" t="n">
+        <v>49</v>
       </c>
       <c r="D46" t="n">
         <v>39</v>
@@ -1457,10 +1367,8 @@
       <c r="B47" t="n">
         <v>46</v>
       </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C47" t="n">
+        <v>24</v>
       </c>
       <c r="D47" t="n">
         <v>39</v>
@@ -1479,10 +1387,8 @@
       <c r="B48" t="n">
         <v>47</v>
       </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C48" t="n">
+        <v>50</v>
       </c>
       <c r="D48" t="n">
         <v>40</v>
@@ -1501,10 +1407,8 @@
       <c r="B49" t="n">
         <v>48</v>
       </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C49" t="n">
+        <v>27</v>
       </c>
       <c r="D49" t="n">
         <v>40</v>
@@ -1523,10 +1427,8 @@
       <c r="B50" t="n">
         <v>49</v>
       </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C50" t="n">
+        <v>29</v>
       </c>
       <c r="D50" t="n">
         <v>40</v>
@@ -1545,10 +1447,8 @@
       <c r="B51" t="n">
         <v>50</v>
       </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C51" t="n">
+        <v>31</v>
       </c>
       <c r="D51" t="n">
         <v>40</v>
@@ -1567,10 +1467,8 @@
       <c r="B52" t="n">
         <v>51</v>
       </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C52" t="n">
+        <v>49</v>
       </c>
       <c r="D52" t="n">
         <v>42</v>
@@ -1589,10 +1487,8 @@
       <c r="B53" t="n">
         <v>52</v>
       </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C53" t="n">
+        <v>33</v>
       </c>
       <c r="D53" t="n">
         <v>42</v>
@@ -1611,10 +1507,8 @@
       <c r="B54" t="n">
         <v>53</v>
       </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C54" t="n">
+        <v>31</v>
       </c>
       <c r="D54" t="n">
         <v>43</v>
@@ -1633,10 +1527,8 @@
       <c r="B55" t="n">
         <v>54</v>
       </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C55" t="n">
+        <v>59</v>
       </c>
       <c r="D55" t="n">
         <v>43</v>
@@ -1655,10 +1547,8 @@
       <c r="B56" t="n">
         <v>55</v>
       </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C56" t="n">
+        <v>50</v>
       </c>
       <c r="D56" t="n">
         <v>43</v>
@@ -1677,10 +1567,8 @@
       <c r="B57" t="n">
         <v>56</v>
       </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C57" t="n">
+        <v>47</v>
       </c>
       <c r="D57" t="n">
         <v>43</v>
@@ -1699,10 +1587,8 @@
       <c r="B58" t="n">
         <v>57</v>
       </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C58" t="n">
+        <v>51</v>
       </c>
       <c r="D58" t="n">
         <v>44</v>
@@ -1721,10 +1607,8 @@
       <c r="B59" t="n">
         <v>58</v>
       </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C59" t="n">
+        <v>69</v>
       </c>
       <c r="D59" t="n">
         <v>44</v>
@@ -1743,10 +1627,8 @@
       <c r="B60" t="n">
         <v>59</v>
       </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C60" t="n">
+        <v>27</v>
       </c>
       <c r="D60" t="n">
         <v>46</v>
@@ -1765,10 +1647,8 @@
       <c r="B61" t="n">
         <v>60</v>
       </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C61" t="n">
+        <v>53</v>
       </c>
       <c r="D61" t="n">
         <v>46</v>
@@ -1787,10 +1667,8 @@
       <c r="B62" t="n">
         <v>61</v>
       </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C62" t="n">
+        <v>70</v>
       </c>
       <c r="D62" t="n">
         <v>46</v>
@@ -1809,10 +1687,8 @@
       <c r="B63" t="n">
         <v>62</v>
       </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C63" t="n">
+        <v>19</v>
       </c>
       <c r="D63" t="n">
         <v>46</v>
@@ -1831,10 +1707,8 @@
       <c r="B64" t="n">
         <v>63</v>
       </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C64" t="n">
+        <v>67</v>
       </c>
       <c r="D64" t="n">
         <v>47</v>
@@ -1853,10 +1727,8 @@
       <c r="B65" t="n">
         <v>64</v>
       </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C65" t="n">
+        <v>54</v>
       </c>
       <c r="D65" t="n">
         <v>47</v>
@@ -1875,10 +1747,8 @@
       <c r="B66" t="n">
         <v>65</v>
       </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C66" t="n">
+        <v>63</v>
       </c>
       <c r="D66" t="n">
         <v>48</v>
@@ -1897,10 +1767,8 @@
       <c r="B67" t="n">
         <v>66</v>
       </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C67" t="n">
+        <v>18</v>
       </c>
       <c r="D67" t="n">
         <v>48</v>
@@ -1919,10 +1787,8 @@
       <c r="B68" t="n">
         <v>67</v>
       </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C68" t="n">
+        <v>43</v>
       </c>
       <c r="D68" t="n">
         <v>48</v>
@@ -1941,10 +1807,8 @@
       <c r="B69" t="n">
         <v>68</v>
       </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C69" t="n">
+        <v>68</v>
       </c>
       <c r="D69" t="n">
         <v>48</v>
@@ -1963,10 +1827,8 @@
       <c r="B70" t="n">
         <v>69</v>
       </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C70" t="n">
+        <v>19</v>
       </c>
       <c r="D70" t="n">
         <v>48</v>
@@ -1985,10 +1847,8 @@
       <c r="B71" t="n">
         <v>70</v>
       </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C71" t="n">
+        <v>32</v>
       </c>
       <c r="D71" t="n">
         <v>48</v>
@@ -2007,10 +1867,8 @@
       <c r="B72" t="n">
         <v>71</v>
       </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C72" t="n">
+        <v>70</v>
       </c>
       <c r="D72" t="n">
         <v>49</v>
@@ -2029,10 +1887,8 @@
       <c r="B73" t="n">
         <v>72</v>
       </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C73" t="n">
+        <v>47</v>
       </c>
       <c r="D73" t="n">
         <v>49</v>
@@ -2051,10 +1907,8 @@
       <c r="B74" t="n">
         <v>73</v>
       </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C74" t="n">
+        <v>60</v>
       </c>
       <c r="D74" t="n">
         <v>50</v>
@@ -2073,10 +1927,8 @@
       <c r="B75" t="n">
         <v>74</v>
       </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C75" t="n">
+        <v>60</v>
       </c>
       <c r="D75" t="n">
         <v>50</v>
@@ -2095,10 +1947,8 @@
       <c r="B76" t="n">
         <v>75</v>
       </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C76" t="n">
+        <v>59</v>
       </c>
       <c r="D76" t="n">
         <v>54</v>
@@ -2117,10 +1967,8 @@
       <c r="B77" t="n">
         <v>76</v>
       </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C77" t="n">
+        <v>26</v>
       </c>
       <c r="D77" t="n">
         <v>54</v>
@@ -2139,10 +1987,8 @@
       <c r="B78" t="n">
         <v>77</v>
       </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C78" t="n">
+        <v>45</v>
       </c>
       <c r="D78" t="n">
         <v>54</v>
@@ -2161,10 +2007,8 @@
       <c r="B79" t="n">
         <v>78</v>
       </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C79" t="n">
+        <v>40</v>
       </c>
       <c r="D79" t="n">
         <v>54</v>
@@ -2183,10 +2027,8 @@
       <c r="B80" t="n">
         <v>79</v>
       </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C80" t="n">
+        <v>23</v>
       </c>
       <c r="D80" t="n">
         <v>54</v>
@@ -2205,10 +2047,8 @@
       <c r="B81" t="n">
         <v>80</v>
       </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C81" t="n">
+        <v>49</v>
       </c>
       <c r="D81" t="n">
         <v>54</v>
@@ -2227,10 +2067,8 @@
       <c r="B82" t="n">
         <v>81</v>
       </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C82" t="n">
+        <v>57</v>
       </c>
       <c r="D82" t="n">
         <v>54</v>
@@ -2249,10 +2087,8 @@
       <c r="B83" t="n">
         <v>82</v>
       </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C83" t="n">
+        <v>38</v>
       </c>
       <c r="D83" t="n">
         <v>54</v>
@@ -2271,10 +2107,8 @@
       <c r="B84" t="n">
         <v>83</v>
       </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C84" t="n">
+        <v>67</v>
       </c>
       <c r="D84" t="n">
         <v>54</v>
@@ -2293,10 +2127,8 @@
       <c r="B85" t="n">
         <v>84</v>
       </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C85" t="n">
+        <v>46</v>
       </c>
       <c r="D85" t="n">
         <v>54</v>
@@ -2315,10 +2147,8 @@
       <c r="B86" t="n">
         <v>85</v>
       </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C86" t="n">
+        <v>21</v>
       </c>
       <c r="D86" t="n">
         <v>54</v>
@@ -2337,10 +2167,8 @@
       <c r="B87" t="n">
         <v>86</v>
       </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C87" t="n">
+        <v>48</v>
       </c>
       <c r="D87" t="n">
         <v>54</v>
@@ -2359,10 +2187,8 @@
       <c r="B88" t="n">
         <v>87</v>
       </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C88" t="n">
+        <v>55</v>
       </c>
       <c r="D88" t="n">
         <v>57</v>
@@ -2381,10 +2207,8 @@
       <c r="B89" t="n">
         <v>88</v>
       </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C89" t="n">
+        <v>22</v>
       </c>
       <c r="D89" t="n">
         <v>57</v>
@@ -2403,10 +2227,8 @@
       <c r="B90" t="n">
         <v>89</v>
       </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C90" t="n">
+        <v>34</v>
       </c>
       <c r="D90" t="n">
         <v>58</v>
@@ -2425,10 +2247,8 @@
       <c r="B91" t="n">
         <v>90</v>
       </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C91" t="n">
+        <v>50</v>
       </c>
       <c r="D91" t="n">
         <v>58</v>
@@ -2447,10 +2267,8 @@
       <c r="B92" t="n">
         <v>91</v>
       </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C92" t="n">
+        <v>68</v>
       </c>
       <c r="D92" t="n">
         <v>59</v>
@@ -2469,10 +2287,8 @@
       <c r="B93" t="n">
         <v>92</v>
       </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C93" t="n">
+        <v>18</v>
       </c>
       <c r="D93" t="n">
         <v>59</v>
@@ -2491,10 +2307,8 @@
       <c r="B94" t="n">
         <v>93</v>
       </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C94" t="n">
+        <v>48</v>
       </c>
       <c r="D94" t="n">
         <v>60</v>
@@ -2513,10 +2327,8 @@
       <c r="B95" t="n">
         <v>94</v>
       </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C95" t="n">
+        <v>40</v>
       </c>
       <c r="D95" t="n">
         <v>60</v>
@@ -2535,10 +2347,8 @@
       <c r="B96" t="n">
         <v>95</v>
       </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C96" t="n">
+        <v>32</v>
       </c>
       <c r="D96" t="n">
         <v>60</v>
@@ -2557,10 +2367,8 @@
       <c r="B97" t="n">
         <v>96</v>
       </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C97" t="n">
+        <v>24</v>
       </c>
       <c r="D97" t="n">
         <v>60</v>
@@ -2579,10 +2387,8 @@
       <c r="B98" t="n">
         <v>97</v>
       </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C98" t="n">
+        <v>47</v>
       </c>
       <c r="D98" t="n">
         <v>60</v>
@@ -2601,10 +2407,8 @@
       <c r="B99" t="n">
         <v>98</v>
       </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C99" t="n">
+        <v>27</v>
       </c>
       <c r="D99" t="n">
         <v>60</v>
@@ -2623,10 +2427,8 @@
       <c r="B100" t="n">
         <v>99</v>
       </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C100" t="n">
+        <v>48</v>
       </c>
       <c r="D100" t="n">
         <v>61</v>
@@ -2645,10 +2447,8 @@
       <c r="B101" t="n">
         <v>100</v>
       </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C101" t="n">
+        <v>20</v>
       </c>
       <c r="D101" t="n">
         <v>61</v>
@@ -2667,10 +2467,8 @@
       <c r="B102" t="n">
         <v>101</v>
       </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C102" t="n">
+        <v>23</v>
       </c>
       <c r="D102" t="n">
         <v>62</v>
@@ -2689,10 +2487,8 @@
       <c r="B103" t="n">
         <v>102</v>
       </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C103" t="n">
+        <v>49</v>
       </c>
       <c r="D103" t="n">
         <v>62</v>
@@ -2711,10 +2507,8 @@
       <c r="B104" t="n">
         <v>103</v>
       </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C104" t="n">
+        <v>67</v>
       </c>
       <c r="D104" t="n">
         <v>62</v>
@@ -2733,10 +2527,8 @@
       <c r="B105" t="n">
         <v>104</v>
       </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C105" t="n">
+        <v>26</v>
       </c>
       <c r="D105" t="n">
         <v>62</v>
@@ -2755,10 +2547,8 @@
       <c r="B106" t="n">
         <v>105</v>
       </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C106" t="n">
+        <v>49</v>
       </c>
       <c r="D106" t="n">
         <v>62</v>
@@ -2777,10 +2567,8 @@
       <c r="B107" t="n">
         <v>106</v>
       </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C107" t="n">
+        <v>21</v>
       </c>
       <c r="D107" t="n">
         <v>62</v>
@@ -2799,10 +2587,8 @@
       <c r="B108" t="n">
         <v>107</v>
       </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C108" t="n">
+        <v>66</v>
       </c>
       <c r="D108" t="n">
         <v>63</v>
@@ -2821,10 +2607,8 @@
       <c r="B109" t="n">
         <v>108</v>
       </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C109" t="n">
+        <v>54</v>
       </c>
       <c r="D109" t="n">
         <v>63</v>
@@ -2843,10 +2627,8 @@
       <c r="B110" t="n">
         <v>109</v>
       </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C110" t="n">
+        <v>68</v>
       </c>
       <c r="D110" t="n">
         <v>63</v>
@@ -2865,10 +2647,8 @@
       <c r="B111" t="n">
         <v>110</v>
       </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C111" t="n">
+        <v>66</v>
       </c>
       <c r="D111" t="n">
         <v>63</v>
@@ -2887,10 +2667,8 @@
       <c r="B112" t="n">
         <v>111</v>
       </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C112" t="n">
+        <v>65</v>
       </c>
       <c r="D112" t="n">
         <v>63</v>
@@ -2909,10 +2687,8 @@
       <c r="B113" t="n">
         <v>112</v>
       </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C113" t="n">
+        <v>19</v>
       </c>
       <c r="D113" t="n">
         <v>63</v>
@@ -2931,10 +2707,8 @@
       <c r="B114" t="n">
         <v>113</v>
       </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C114" t="n">
+        <v>38</v>
       </c>
       <c r="D114" t="n">
         <v>64</v>
@@ -2953,10 +2727,8 @@
       <c r="B115" t="n">
         <v>114</v>
       </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C115" t="n">
+        <v>19</v>
       </c>
       <c r="D115" t="n">
         <v>64</v>
@@ -2975,10 +2747,8 @@
       <c r="B116" t="n">
         <v>115</v>
       </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C116" t="n">
+        <v>18</v>
       </c>
       <c r="D116" t="n">
         <v>65</v>
@@ -2997,10 +2767,8 @@
       <c r="B117" t="n">
         <v>116</v>
       </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C117" t="n">
+        <v>19</v>
       </c>
       <c r="D117" t="n">
         <v>65</v>
@@ -3019,10 +2787,8 @@
       <c r="B118" t="n">
         <v>117</v>
       </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C118" t="n">
+        <v>63</v>
       </c>
       <c r="D118" t="n">
         <v>65</v>
@@ -3041,10 +2807,8 @@
       <c r="B119" t="n">
         <v>118</v>
       </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C119" t="n">
+        <v>49</v>
       </c>
       <c r="D119" t="n">
         <v>65</v>
@@ -3063,10 +2827,8 @@
       <c r="B120" t="n">
         <v>119</v>
       </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C120" t="n">
+        <v>51</v>
       </c>
       <c r="D120" t="n">
         <v>67</v>
@@ -3085,10 +2847,8 @@
       <c r="B121" t="n">
         <v>120</v>
       </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C121" t="n">
+        <v>50</v>
       </c>
       <c r="D121" t="n">
         <v>67</v>
@@ -3107,10 +2867,8 @@
       <c r="B122" t="n">
         <v>121</v>
       </c>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C122" t="n">
+        <v>27</v>
       </c>
       <c r="D122" t="n">
         <v>67</v>
@@ -3129,10 +2887,8 @@
       <c r="B123" t="n">
         <v>122</v>
       </c>
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C123" t="n">
+        <v>38</v>
       </c>
       <c r="D123" t="n">
         <v>67</v>
@@ -3151,10 +2907,8 @@
       <c r="B124" t="n">
         <v>123</v>
       </c>
-      <c r="C124" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C124" t="n">
+        <v>40</v>
       </c>
       <c r="D124" t="n">
         <v>69</v>
@@ -3173,10 +2927,8 @@
       <c r="B125" t="n">
         <v>124</v>
       </c>
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C125" t="n">
+        <v>39</v>
       </c>
       <c r="D125" t="n">
         <v>69</v>
@@ -3185,7 +2937,7 @@
         <v>91</v>
       </c>
       <c r="F125" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="126">
@@ -3195,10 +2947,8 @@
       <c r="B126" t="n">
         <v>125</v>
       </c>
-      <c r="C126" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C126" t="n">
+        <v>23</v>
       </c>
       <c r="D126" t="n">
         <v>70</v>
@@ -3217,10 +2967,8 @@
       <c r="B127" t="n">
         <v>126</v>
       </c>
-      <c r="C127" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C127" t="n">
+        <v>31</v>
       </c>
       <c r="D127" t="n">
         <v>70</v>
@@ -3229,7 +2977,7 @@
         <v>77</v>
       </c>
       <c r="F127" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128">
@@ -3239,10 +2987,8 @@
       <c r="B128" t="n">
         <v>127</v>
       </c>
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C128" t="n">
+        <v>43</v>
       </c>
       <c r="D128" t="n">
         <v>71</v>
@@ -3261,10 +3007,8 @@
       <c r="B129" t="n">
         <v>128</v>
       </c>
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C129" t="n">
+        <v>40</v>
       </c>
       <c r="D129" t="n">
         <v>71</v>
@@ -3273,7 +3017,7 @@
         <v>95</v>
       </c>
       <c r="F129" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130">
@@ -3283,10 +3027,8 @@
       <c r="B130" t="n">
         <v>129</v>
       </c>
-      <c r="C130" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C130" t="n">
+        <v>59</v>
       </c>
       <c r="D130" t="n">
         <v>71</v>
@@ -3295,7 +3037,7 @@
         <v>11</v>
       </c>
       <c r="F130" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131">
@@ -3305,10 +3047,8 @@
       <c r="B131" t="n">
         <v>130</v>
       </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C131" t="n">
+        <v>38</v>
       </c>
       <c r="D131" t="n">
         <v>71</v>
@@ -3317,7 +3057,7 @@
         <v>75</v>
       </c>
       <c r="F131" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="132">
@@ -3327,10 +3067,8 @@
       <c r="B132" t="n">
         <v>131</v>
       </c>
-      <c r="C132" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C132" t="n">
+        <v>47</v>
       </c>
       <c r="D132" t="n">
         <v>71</v>
@@ -3339,7 +3077,7 @@
         <v>9</v>
       </c>
       <c r="F132" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133">
@@ -3349,10 +3087,8 @@
       <c r="B133" t="n">
         <v>132</v>
       </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C133" t="n">
+        <v>39</v>
       </c>
       <c r="D133" t="n">
         <v>71</v>
@@ -3361,7 +3097,7 @@
         <v>75</v>
       </c>
       <c r="F133" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134">
@@ -3371,10 +3107,8 @@
       <c r="B134" t="n">
         <v>133</v>
       </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C134" t="n">
+        <v>25</v>
       </c>
       <c r="D134" t="n">
         <v>72</v>
@@ -3393,10 +3127,8 @@
       <c r="B135" t="n">
         <v>134</v>
       </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C135" t="n">
+        <v>31</v>
       </c>
       <c r="D135" t="n">
         <v>72</v>
@@ -3405,7 +3137,7 @@
         <v>71</v>
       </c>
       <c r="F135" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="136">
@@ -3415,10 +3147,8 @@
       <c r="B136" t="n">
         <v>135</v>
       </c>
-      <c r="C136" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C136" t="n">
+        <v>20</v>
       </c>
       <c r="D136" t="n">
         <v>73</v>
@@ -3427,7 +3157,7 @@
         <v>5</v>
       </c>
       <c r="F136" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="137">
@@ -3437,10 +3167,8 @@
       <c r="B137" t="n">
         <v>136</v>
       </c>
-      <c r="C137" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C137" t="n">
+        <v>29</v>
       </c>
       <c r="D137" t="n">
         <v>73</v>
@@ -3449,7 +3177,7 @@
         <v>88</v>
       </c>
       <c r="F137" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138">
@@ -3459,10 +3187,8 @@
       <c r="B138" t="n">
         <v>137</v>
       </c>
-      <c r="C138" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C138" t="n">
+        <v>44</v>
       </c>
       <c r="D138" t="n">
         <v>73</v>
@@ -3471,7 +3197,7 @@
         <v>7</v>
       </c>
       <c r="F138" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139">
@@ -3481,10 +3207,8 @@
       <c r="B139" t="n">
         <v>138</v>
       </c>
-      <c r="C139" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C139" t="n">
+        <v>32</v>
       </c>
       <c r="D139" t="n">
         <v>73</v>
@@ -3493,7 +3217,7 @@
         <v>73</v>
       </c>
       <c r="F139" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="140">
@@ -3503,10 +3227,8 @@
       <c r="B140" t="n">
         <v>139</v>
       </c>
-      <c r="C140" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C140" t="n">
+        <v>19</v>
       </c>
       <c r="D140" t="n">
         <v>74</v>
@@ -3515,7 +3237,7 @@
         <v>10</v>
       </c>
       <c r="F140" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="141">
@@ -3525,10 +3247,8 @@
       <c r="B141" t="n">
         <v>140</v>
       </c>
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C141" t="n">
+        <v>35</v>
       </c>
       <c r="D141" t="n">
         <v>74</v>
@@ -3537,7 +3257,7 @@
         <v>72</v>
       </c>
       <c r="F141" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142">
@@ -3547,10 +3267,8 @@
       <c r="B142" t="n">
         <v>141</v>
       </c>
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C142" t="n">
+        <v>57</v>
       </c>
       <c r="D142" t="n">
         <v>75</v>
@@ -3559,7 +3277,7 @@
         <v>5</v>
       </c>
       <c r="F142" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143">
@@ -3569,10 +3287,8 @@
       <c r="B143" t="n">
         <v>142</v>
       </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C143" t="n">
+        <v>32</v>
       </c>
       <c r="D143" t="n">
         <v>75</v>
@@ -3581,7 +3297,7 @@
         <v>93</v>
       </c>
       <c r="F143" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144">
@@ -3591,10 +3307,8 @@
       <c r="B144" t="n">
         <v>143</v>
       </c>
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C144" t="n">
+        <v>28</v>
       </c>
       <c r="D144" t="n">
         <v>76</v>
@@ -3613,10 +3327,8 @@
       <c r="B145" t="n">
         <v>144</v>
       </c>
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C145" t="n">
+        <v>32</v>
       </c>
       <c r="D145" t="n">
         <v>76</v>
@@ -3625,7 +3337,7 @@
         <v>87</v>
       </c>
       <c r="F145" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146">
@@ -3635,10 +3347,8 @@
       <c r="B146" t="n">
         <v>145</v>
       </c>
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C146" t="n">
+        <v>25</v>
       </c>
       <c r="D146" t="n">
         <v>77</v>
@@ -3647,7 +3357,7 @@
         <v>12</v>
       </c>
       <c r="F146" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="147">
@@ -3657,10 +3367,8 @@
       <c r="B147" t="n">
         <v>146</v>
       </c>
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C147" t="n">
+        <v>28</v>
       </c>
       <c r="D147" t="n">
         <v>77</v>
@@ -3669,7 +3377,7 @@
         <v>97</v>
       </c>
       <c r="F147" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148">
@@ -3679,10 +3387,8 @@
       <c r="B148" t="n">
         <v>147</v>
       </c>
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C148" t="n">
+        <v>48</v>
       </c>
       <c r="D148" t="n">
         <v>77</v>
@@ -3701,10 +3407,8 @@
       <c r="B149" t="n">
         <v>148</v>
       </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C149" t="n">
+        <v>32</v>
       </c>
       <c r="D149" t="n">
         <v>77</v>
@@ -3713,7 +3417,7 @@
         <v>74</v>
       </c>
       <c r="F149" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150">
@@ -3723,10 +3427,8 @@
       <c r="B150" t="n">
         <v>149</v>
       </c>
-      <c r="C150" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C150" t="n">
+        <v>34</v>
       </c>
       <c r="D150" t="n">
         <v>78</v>
@@ -3735,7 +3437,7 @@
         <v>22</v>
       </c>
       <c r="F150" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="151">
@@ -3745,10 +3447,8 @@
       <c r="B151" t="n">
         <v>150</v>
       </c>
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C151" t="n">
+        <v>34</v>
       </c>
       <c r="D151" t="n">
         <v>78</v>
@@ -3757,7 +3457,7 @@
         <v>90</v>
       </c>
       <c r="F151" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152">
@@ -3767,10 +3467,8 @@
       <c r="B152" t="n">
         <v>151</v>
       </c>
-      <c r="C152" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C152" t="n">
+        <v>43</v>
       </c>
       <c r="D152" t="n">
         <v>78</v>
@@ -3779,7 +3477,7 @@
         <v>17</v>
       </c>
       <c r="F152" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="153">
@@ -3789,10 +3487,8 @@
       <c r="B153" t="n">
         <v>152</v>
       </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C153" t="n">
+        <v>39</v>
       </c>
       <c r="D153" t="n">
         <v>78</v>
@@ -3801,7 +3497,7 @@
         <v>88</v>
       </c>
       <c r="F153" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="154">
@@ -3811,10 +3507,8 @@
       <c r="B154" t="n">
         <v>153</v>
       </c>
-      <c r="C154" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C154" t="n">
+        <v>44</v>
       </c>
       <c r="D154" t="n">
         <v>78</v>
@@ -3823,7 +3517,7 @@
         <v>20</v>
       </c>
       <c r="F154" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="155">
@@ -3833,10 +3527,8 @@
       <c r="B155" t="n">
         <v>154</v>
       </c>
-      <c r="C155" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C155" t="n">
+        <v>38</v>
       </c>
       <c r="D155" t="n">
         <v>78</v>
@@ -3845,7 +3537,7 @@
         <v>76</v>
       </c>
       <c r="F155" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156">
@@ -3855,10 +3547,8 @@
       <c r="B156" t="n">
         <v>155</v>
       </c>
-      <c r="C156" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C156" t="n">
+        <v>47</v>
       </c>
       <c r="D156" t="n">
         <v>78</v>
@@ -3867,7 +3557,7 @@
         <v>16</v>
       </c>
       <c r="F156" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="157">
@@ -3877,10 +3567,8 @@
       <c r="B157" t="n">
         <v>156</v>
       </c>
-      <c r="C157" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C157" t="n">
+        <v>27</v>
       </c>
       <c r="D157" t="n">
         <v>78</v>
@@ -3889,7 +3577,7 @@
         <v>89</v>
       </c>
       <c r="F157" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="158">
@@ -3899,10 +3587,8 @@
       <c r="B158" t="n">
         <v>157</v>
       </c>
-      <c r="C158" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C158" t="n">
+        <v>37</v>
       </c>
       <c r="D158" t="n">
         <v>78</v>
@@ -3911,7 +3597,7 @@
         <v>1</v>
       </c>
       <c r="F158" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="159">
@@ -3921,10 +3607,8 @@
       <c r="B159" t="n">
         <v>158</v>
       </c>
-      <c r="C159" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C159" t="n">
+        <v>30</v>
       </c>
       <c r="D159" t="n">
         <v>78</v>
@@ -3933,7 +3617,7 @@
         <v>78</v>
       </c>
       <c r="F159" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="160">
@@ -3943,10 +3627,8 @@
       <c r="B160" t="n">
         <v>159</v>
       </c>
-      <c r="C160" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C160" t="n">
+        <v>34</v>
       </c>
       <c r="D160" t="n">
         <v>78</v>
@@ -3955,7 +3637,7 @@
         <v>1</v>
       </c>
       <c r="F160" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="161">
@@ -3965,10 +3647,8 @@
       <c r="B161" t="n">
         <v>160</v>
       </c>
-      <c r="C161" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C161" t="n">
+        <v>30</v>
       </c>
       <c r="D161" t="n">
         <v>78</v>
@@ -3977,7 +3657,7 @@
         <v>73</v>
       </c>
       <c r="F161" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="162">
@@ -3987,10 +3667,8 @@
       <c r="B162" t="n">
         <v>161</v>
       </c>
-      <c r="C162" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C162" t="n">
+        <v>56</v>
       </c>
       <c r="D162" t="n">
         <v>79</v>
@@ -4009,10 +3687,8 @@
       <c r="B163" t="n">
         <v>162</v>
       </c>
-      <c r="C163" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C163" t="n">
+        <v>29</v>
       </c>
       <c r="D163" t="n">
         <v>79</v>
@@ -4021,7 +3697,7 @@
         <v>83</v>
       </c>
       <c r="F163" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="164">
@@ -4031,10 +3707,8 @@
       <c r="B164" t="n">
         <v>163</v>
       </c>
-      <c r="C164" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C164" t="n">
+        <v>19</v>
       </c>
       <c r="D164" t="n">
         <v>81</v>
@@ -4043,7 +3717,7 @@
         <v>5</v>
       </c>
       <c r="F164" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="165">
@@ -4053,10 +3727,8 @@
       <c r="B165" t="n">
         <v>164</v>
       </c>
-      <c r="C165" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C165" t="n">
+        <v>31</v>
       </c>
       <c r="D165" t="n">
         <v>81</v>
@@ -4065,7 +3737,7 @@
         <v>93</v>
       </c>
       <c r="F165" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="166">
@@ -4075,10 +3747,8 @@
       <c r="B166" t="n">
         <v>165</v>
       </c>
-      <c r="C166" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C166" t="n">
+        <v>50</v>
       </c>
       <c r="D166" t="n">
         <v>85</v>
@@ -4087,7 +3757,7 @@
         <v>26</v>
       </c>
       <c r="F166" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="167">
@@ -4097,10 +3767,8 @@
       <c r="B167" t="n">
         <v>166</v>
       </c>
-      <c r="C167" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C167" t="n">
+        <v>36</v>
       </c>
       <c r="D167" t="n">
         <v>85</v>
@@ -4109,7 +3777,7 @@
         <v>75</v>
       </c>
       <c r="F167" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="168">
@@ -4119,10 +3787,8 @@
       <c r="B168" t="n">
         <v>167</v>
       </c>
-      <c r="C168" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C168" t="n">
+        <v>42</v>
       </c>
       <c r="D168" t="n">
         <v>86</v>
@@ -4131,7 +3797,7 @@
         <v>20</v>
       </c>
       <c r="F168" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="169">
@@ -4141,10 +3807,8 @@
       <c r="B169" t="n">
         <v>168</v>
       </c>
-      <c r="C169" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C169" t="n">
+        <v>33</v>
       </c>
       <c r="D169" t="n">
         <v>86</v>
@@ -4153,7 +3817,7 @@
         <v>95</v>
       </c>
       <c r="F169" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="170">
@@ -4163,10 +3827,8 @@
       <c r="B170" t="n">
         <v>169</v>
       </c>
-      <c r="C170" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C170" t="n">
+        <v>36</v>
       </c>
       <c r="D170" t="n">
         <v>87</v>
@@ -4175,7 +3837,7 @@
         <v>27</v>
       </c>
       <c r="F170" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="171">
@@ -4185,10 +3847,8 @@
       <c r="B171" t="n">
         <v>170</v>
       </c>
-      <c r="C171" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C171" t="n">
+        <v>32</v>
       </c>
       <c r="D171" t="n">
         <v>87</v>
@@ -4197,7 +3857,7 @@
         <v>63</v>
       </c>
       <c r="F171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="172">
@@ -4207,10 +3867,8 @@
       <c r="B172" t="n">
         <v>171</v>
       </c>
-      <c r="C172" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C172" t="n">
+        <v>40</v>
       </c>
       <c r="D172" t="n">
         <v>87</v>
@@ -4219,7 +3877,7 @@
         <v>13</v>
       </c>
       <c r="F172" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="173">
@@ -4229,10 +3887,8 @@
       <c r="B173" t="n">
         <v>172</v>
       </c>
-      <c r="C173" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C173" t="n">
+        <v>28</v>
       </c>
       <c r="D173" t="n">
         <v>87</v>
@@ -4241,7 +3897,7 @@
         <v>75</v>
       </c>
       <c r="F173" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="174">
@@ -4251,10 +3907,8 @@
       <c r="B174" t="n">
         <v>173</v>
       </c>
-      <c r="C174" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C174" t="n">
+        <v>36</v>
       </c>
       <c r="D174" t="n">
         <v>87</v>
@@ -4263,7 +3917,7 @@
         <v>10</v>
       </c>
       <c r="F174" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="175">
@@ -4273,10 +3927,8 @@
       <c r="B175" t="n">
         <v>174</v>
       </c>
-      <c r="C175" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C175" t="n">
+        <v>36</v>
       </c>
       <c r="D175" t="n">
         <v>87</v>
@@ -4285,7 +3937,7 @@
         <v>92</v>
       </c>
       <c r="F175" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="176">
@@ -4295,10 +3947,8 @@
       <c r="B176" t="n">
         <v>175</v>
       </c>
-      <c r="C176" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C176" t="n">
+        <v>52</v>
       </c>
       <c r="D176" t="n">
         <v>88</v>
@@ -4307,7 +3957,7 @@
         <v>13</v>
       </c>
       <c r="F176" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="177">
@@ -4317,10 +3967,8 @@
       <c r="B177" t="n">
         <v>176</v>
       </c>
-      <c r="C177" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C177" t="n">
+        <v>30</v>
       </c>
       <c r="D177" t="n">
         <v>88</v>
@@ -4329,7 +3977,7 @@
         <v>86</v>
       </c>
       <c r="F177" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178">
@@ -4339,10 +3987,8 @@
       <c r="B178" t="n">
         <v>177</v>
       </c>
-      <c r="C178" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C178" t="n">
+        <v>58</v>
       </c>
       <c r="D178" t="n">
         <v>88</v>
@@ -4351,7 +3997,7 @@
         <v>15</v>
       </c>
       <c r="F178" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="179">
@@ -4361,10 +4007,8 @@
       <c r="B179" t="n">
         <v>178</v>
       </c>
-      <c r="C179" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C179" t="n">
+        <v>27</v>
       </c>
       <c r="D179" t="n">
         <v>88</v>
@@ -4373,7 +4017,7 @@
         <v>69</v>
       </c>
       <c r="F179" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="180">
@@ -4383,10 +4027,8 @@
       <c r="B180" t="n">
         <v>179</v>
       </c>
-      <c r="C180" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C180" t="n">
+        <v>59</v>
       </c>
       <c r="D180" t="n">
         <v>93</v>
@@ -4395,7 +4037,7 @@
         <v>14</v>
       </c>
       <c r="F180" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="181">
@@ -4405,10 +4047,8 @@
       <c r="B181" t="n">
         <v>180</v>
       </c>
-      <c r="C181" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C181" t="n">
+        <v>35</v>
       </c>
       <c r="D181" t="n">
         <v>93</v>
@@ -4417,7 +4057,7 @@
         <v>90</v>
       </c>
       <c r="F181" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="182">
@@ -4427,10 +4067,8 @@
       <c r="B182" t="n">
         <v>181</v>
       </c>
-      <c r="C182" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C182" t="n">
+        <v>37</v>
       </c>
       <c r="D182" t="n">
         <v>97</v>
@@ -4439,7 +4077,7 @@
         <v>32</v>
       </c>
       <c r="F182" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="183">
@@ -4449,10 +4087,8 @@
       <c r="B183" t="n">
         <v>182</v>
       </c>
-      <c r="C183" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C183" t="n">
+        <v>32</v>
       </c>
       <c r="D183" t="n">
         <v>97</v>
@@ -4461,7 +4097,7 @@
         <v>86</v>
       </c>
       <c r="F183" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="184">
@@ -4471,10 +4107,8 @@
       <c r="B184" t="n">
         <v>183</v>
       </c>
-      <c r="C184" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C184" t="n">
+        <v>46</v>
       </c>
       <c r="D184" t="n">
         <v>98</v>
@@ -4483,7 +4117,7 @@
         <v>15</v>
       </c>
       <c r="F184" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="185">
@@ -4493,10 +4127,8 @@
       <c r="B185" t="n">
         <v>184</v>
       </c>
-      <c r="C185" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C185" t="n">
+        <v>29</v>
       </c>
       <c r="D185" t="n">
         <v>98</v>
@@ -4505,7 +4137,7 @@
         <v>88</v>
       </c>
       <c r="F185" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="186">
@@ -4515,10 +4147,8 @@
       <c r="B186" t="n">
         <v>185</v>
       </c>
-      <c r="C186" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C186" t="n">
+        <v>41</v>
       </c>
       <c r="D186" t="n">
         <v>99</v>
@@ -4527,7 +4157,7 @@
         <v>39</v>
       </c>
       <c r="F186" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="187">
@@ -4537,10 +4167,8 @@
       <c r="B187" t="n">
         <v>186</v>
       </c>
-      <c r="C187" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C187" t="n">
+        <v>30</v>
       </c>
       <c r="D187" t="n">
         <v>99</v>
@@ -4549,7 +4177,7 @@
         <v>97</v>
       </c>
       <c r="F187" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="188">
@@ -4559,10 +4187,8 @@
       <c r="B188" t="n">
         <v>187</v>
       </c>
-      <c r="C188" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C188" t="n">
+        <v>54</v>
       </c>
       <c r="D188" t="n">
         <v>101</v>
@@ -4571,7 +4197,7 @@
         <v>24</v>
       </c>
       <c r="F188" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="189">
@@ -4581,10 +4207,8 @@
       <c r="B189" t="n">
         <v>188</v>
       </c>
-      <c r="C189" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C189" t="n">
+        <v>28</v>
       </c>
       <c r="D189" t="n">
         <v>101</v>
@@ -4593,7 +4217,7 @@
         <v>68</v>
       </c>
       <c r="F189" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="190">
@@ -4603,10 +4227,8 @@
       <c r="B190" t="n">
         <v>189</v>
       </c>
-      <c r="C190" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C190" t="n">
+        <v>41</v>
       </c>
       <c r="D190" t="n">
         <v>103</v>
@@ -4615,7 +4237,7 @@
         <v>17</v>
       </c>
       <c r="F190" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="191">
@@ -4625,10 +4247,8 @@
       <c r="B191" t="n">
         <v>190</v>
       </c>
-      <c r="C191" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C191" t="n">
+        <v>36</v>
       </c>
       <c r="D191" t="n">
         <v>103</v>
@@ -4637,7 +4257,7 @@
         <v>85</v>
       </c>
       <c r="F191" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="192">
@@ -4647,10 +4267,8 @@
       <c r="B192" t="n">
         <v>191</v>
       </c>
-      <c r="C192" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C192" t="n">
+        <v>34</v>
       </c>
       <c r="D192" t="n">
         <v>103</v>
@@ -4659,7 +4277,7 @@
         <v>23</v>
       </c>
       <c r="F192" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="193">
@@ -4669,10 +4287,8 @@
       <c r="B193" t="n">
         <v>192</v>
       </c>
-      <c r="C193" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C193" t="n">
+        <v>32</v>
       </c>
       <c r="D193" t="n">
         <v>103</v>
@@ -4681,7 +4297,7 @@
         <v>69</v>
       </c>
       <c r="F193" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="194">
@@ -4691,10 +4307,8 @@
       <c r="B194" t="n">
         <v>193</v>
       </c>
-      <c r="C194" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C194" t="n">
+        <v>33</v>
       </c>
       <c r="D194" t="n">
         <v>113</v>
@@ -4703,7 +4317,7 @@
         <v>8</v>
       </c>
       <c r="F194" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="195">
@@ -4713,10 +4327,8 @@
       <c r="B195" t="n">
         <v>194</v>
       </c>
-      <c r="C195" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C195" t="n">
+        <v>38</v>
       </c>
       <c r="D195" t="n">
         <v>113</v>
@@ -4725,7 +4337,7 @@
         <v>91</v>
       </c>
       <c r="F195" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="196">
@@ -4735,10 +4347,8 @@
       <c r="B196" t="n">
         <v>195</v>
       </c>
-      <c r="C196" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C196" t="n">
+        <v>47</v>
       </c>
       <c r="D196" t="n">
         <v>120</v>
@@ -4747,7 +4357,7 @@
         <v>16</v>
       </c>
       <c r="F196" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="197">
@@ -4757,10 +4367,8 @@
       <c r="B197" t="n">
         <v>196</v>
       </c>
-      <c r="C197" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C197" t="n">
+        <v>35</v>
       </c>
       <c r="D197" t="n">
         <v>120</v>
@@ -4769,7 +4377,7 @@
         <v>79</v>
       </c>
       <c r="F197" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="198">
@@ -4779,10 +4387,8 @@
       <c r="B198" t="n">
         <v>197</v>
       </c>
-      <c r="C198" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
+      <c r="C198" t="n">
+        <v>45</v>
       </c>
       <c r="D198" t="n">
         <v>126</v>
@@ -4791,7 +4397,7 @@
         <v>28</v>
       </c>
       <c r="F198" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="199">
@@ -4801,10 +4407,8 @@
       <c r="B199" t="n">
         <v>198</v>
       </c>
-      <c r="C199" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C199" t="n">
+        <v>32</v>
       </c>
       <c r="D199" t="n">
         <v>126</v>
@@ -4813,7 +4417,7 @@
         <v>74</v>
       </c>
       <c r="F199" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="200">
@@ -4823,10 +4427,8 @@
       <c r="B200" t="n">
         <v>199</v>
       </c>
-      <c r="C200" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C200" t="n">
+        <v>32</v>
       </c>
       <c r="D200" t="n">
         <v>137</v>
@@ -4835,7 +4437,7 @@
         <v>18</v>
       </c>
       <c r="F200" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="201">
@@ -4845,10 +4447,8 @@
       <c r="B201" t="n">
         <v>200</v>
       </c>
-      <c r="C201" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
+      <c r="C201" t="n">
+        <v>30</v>
       </c>
       <c r="D201" t="n">
         <v>137</v>
@@ -4857,7 +4457,7 @@
         <v>83</v>
       </c>
       <c r="F201" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>